<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@3aca1f614a71989ada6588735e82c06d05241287 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-DiagnoseFreitext.xlsx
+++ b/StructureDefinition-DiagnoseFreitext.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="447">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-17T19:55:11+00:00</t>
+    <t>2024-09-18T10:41:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>Need to track the status of individual results. Some results are finalized before the whole report is finalized.</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
   <si>
     <t>required</t>
@@ -3406,7 +3409,7 @@
         <v>19</v>
       </c>
       <c r="S14" t="s" s="2">
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="T14" t="s" s="2">
         <v>19</v>
@@ -3421,13 +3424,13 @@
         <v>19</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>19</v>
@@ -3460,19 +3463,19 @@
         <v>102</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AO14" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AP14" t="s" s="2">
         <v>19</v>
@@ -3480,10 +3483,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3506,19 +3509,19 @@
         <v>19</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>19</v>
@@ -3546,10 +3549,10 @@
         <v>114</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>19</v>
@@ -3567,7 +3570,7 @@
         <v>19</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>78</v>
@@ -3591,10 +3594,10 @@
         <v>19</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AO15" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AP15" t="s" s="2">
         <v>19</v>
@@ -3602,14 +3605,14 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3628,19 +3631,19 @@
         <v>91</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>19</v>
@@ -3650,7 +3653,7 @@
         <v>19</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="T16" t="s" s="2">
         <v>19</v>
@@ -3665,13 +3668,13 @@
         <v>19</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>19</v>
@@ -3689,7 +3692,7 @@
         <v>19</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>90</v>
@@ -3704,30 +3707,30 @@
         <v>102</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AO16" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AP16" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3750,19 +3753,19 @@
         <v>91</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>19</v>
@@ -3811,7 +3814,7 @@
         <v>19</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>78</v>
@@ -3826,19 +3829,19 @@
         <v>102</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AP17" t="s" s="2">
         <v>19</v>
@@ -3846,10 +3849,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3872,16 +3875,16 @@
         <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3931,7 +3934,7 @@
         <v>19</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>78</v>
@@ -3952,13 +3955,13 @@
         <v>19</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AP18" t="s" s="2">
         <v>19</v>
@@ -3966,14 +3969,14 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
@@ -3992,19 +3995,19 @@
         <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>19</v>
@@ -4053,7 +4056,7 @@
         <v>19</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>78</v>
@@ -4068,19 +4071,19 @@
         <v>102</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="AP19" t="s" s="2">
         <v>19</v>
@@ -4088,14 +4091,14 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -4114,19 +4117,19 @@
         <v>91</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>19</v>
@@ -4175,7 +4178,7 @@
         <v>19</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>78</v>
@@ -4190,19 +4193,19 @@
         <v>102</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AP20" t="s" s="2">
         <v>19</v>
@@ -4210,10 +4213,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4236,16 +4239,16 @@
         <v>91</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -4295,7 +4298,7 @@
         <v>19</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -4316,13 +4319,13 @@
         <v>19</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AP21" t="s" s="2">
         <v>19</v>
@@ -4330,10 +4333,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4356,17 +4359,17 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>19</v>
@@ -4415,7 +4418,7 @@
         <v>19</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -4430,19 +4433,19 @@
         <v>102</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="AP22" t="s" s="2">
         <v>19</v>
@@ -4450,10 +4453,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4476,19 +4479,19 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>19</v>
@@ -4537,7 +4540,7 @@
         <v>19</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -4546,7 +4549,7 @@
         <v>90</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AJ23" t="s" s="2">
         <v>102</v>
@@ -4555,27 +4558,27 @@
         <v>19</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP23" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4598,19 +4601,19 @@
         <v>19</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>19</v>
@@ -4635,13 +4638,13 @@
         <v>19</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Z24" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AA24" t="s" s="2">
         <v>19</v>
@@ -4659,7 +4662,7 @@
         <v>19</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>78</v>
@@ -4668,7 +4671,7 @@
         <v>90</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>102</v>
@@ -4683,7 +4686,7 @@
         <v>133</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>19</v>
@@ -4694,14 +4697,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4720,19 +4723,19 @@
         <v>19</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>19</v>
@@ -4757,13 +4760,13 @@
         <v>19</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>19</v>
@@ -4781,7 +4784,7 @@
         <v>19</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>78</v>
@@ -4799,27 +4802,27 @@
         <v>19</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP25" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4842,19 +4845,19 @@
         <v>19</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>19</v>
@@ -4903,7 +4906,7 @@
         <v>19</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>78</v>
@@ -4924,10 +4927,10 @@
         <v>19</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>19</v>
@@ -4938,10 +4941,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4964,16 +4967,16 @@
         <v>19</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -4999,13 +5002,13 @@
         <v>19</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>19</v>
@@ -5023,7 +5026,7 @@
         <v>19</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>78</v>
@@ -5041,27 +5044,27 @@
         <v>19</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP27" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5084,19 +5087,19 @@
         <v>19</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>19</v>
@@ -5121,13 +5124,13 @@
         <v>19</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>19</v>
@@ -5145,7 +5148,7 @@
         <v>19</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -5166,10 +5169,10 @@
         <v>19</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>19</v>
@@ -5180,10 +5183,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5206,16 +5209,16 @@
         <v>19</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5265,7 +5268,7 @@
         <v>19</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -5283,27 +5286,27 @@
         <v>19</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP29" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5326,16 +5329,16 @@
         <v>19</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
@@ -5385,7 +5388,7 @@
         <v>19</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>78</v>
@@ -5403,27 +5406,27 @@
         <v>19</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP30" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5446,19 +5449,19 @@
         <v>19</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>19</v>
@@ -5507,7 +5510,7 @@
         <v>19</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>78</v>
@@ -5519,7 +5522,7 @@
         <v>19</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>19</v>
@@ -5528,10 +5531,10 @@
         <v>19</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>19</v>
@@ -5542,10 +5545,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5568,13 +5571,13 @@
         <v>19</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5625,7 +5628,7 @@
         <v>19</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>78</v>
@@ -5649,7 +5652,7 @@
         <v>19</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>19</v>
@@ -5660,10 +5663,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5692,7 +5695,7 @@
         <v>137</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="N33" t="s" s="2">
         <v>139</v>
@@ -5745,7 +5748,7 @@
         <v>19</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>78</v>
@@ -5769,7 +5772,7 @@
         <v>19</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>19</v>
@@ -5780,14 +5783,14 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -5809,10 +5812,10 @@
         <v>136</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>139</v>
@@ -5867,7 +5870,7 @@
         <v>19</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>78</v>
@@ -5902,10 +5905,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5928,13 +5931,13 @@
         <v>19</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5985,7 +5988,7 @@
         <v>19</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>78</v>
@@ -5994,7 +5997,7 @@
         <v>90</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>102</v>
@@ -6006,10 +6009,10 @@
         <v>19</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>19</v>
@@ -6020,10 +6023,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6046,13 +6049,13 @@
         <v>19</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6103,7 +6106,7 @@
         <v>19</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -6112,7 +6115,7 @@
         <v>90</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>102</v>
@@ -6124,10 +6127,10 @@
         <v>19</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>19</v>
@@ -6138,10 +6141,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6164,19 +6167,19 @@
         <v>19</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>19</v>
@@ -6204,10 +6207,10 @@
         <v>114</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="Z37" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AA37" t="s" s="2">
         <v>19</v>
@@ -6225,7 +6228,7 @@
         <v>19</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -6243,13 +6246,13 @@
         <v>19</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>19</v>
@@ -6260,10 +6263,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6286,19 +6289,19 @@
         <v>19</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>19</v>
@@ -6323,13 +6326,13 @@
         <v>19</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>19</v>
@@ -6347,7 +6350,7 @@
         <v>19</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -6365,13 +6368,13 @@
         <v>19</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>19</v>
@@ -6382,10 +6385,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6408,17 +6411,17 @@
         <v>19</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>19</v>
@@ -6467,7 +6470,7 @@
         <v>19</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -6491,7 +6494,7 @@
         <v>19</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AO39" t="s" s="2">
         <v>19</v>
@@ -6502,10 +6505,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6528,13 +6531,13 @@
         <v>19</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6585,7 +6588,7 @@
         <v>19</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>78</v>
@@ -6606,10 +6609,10 @@
         <v>19</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>19</v>
@@ -6620,10 +6623,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6646,16 +6649,16 @@
         <v>91</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6705,7 +6708,7 @@
         <v>19</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>78</v>
@@ -6726,10 +6729,10 @@
         <v>19</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>19</v>
@@ -6740,10 +6743,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6766,16 +6769,16 @@
         <v>91</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
@@ -6825,7 +6828,7 @@
         <v>19</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>78</v>
@@ -6846,10 +6849,10 @@
         <v>19</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>19</v>
@@ -6860,10 +6863,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6886,19 +6889,19 @@
         <v>91</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>19</v>
@@ -6947,7 +6950,7 @@
         <v>19</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -6968,10 +6971,10 @@
         <v>19</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>19</v>
@@ -6982,10 +6985,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7008,13 +7011,13 @@
         <v>19</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -7065,7 +7068,7 @@
         <v>19</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -7089,7 +7092,7 @@
         <v>19</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>19</v>
@@ -7100,10 +7103,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7132,7 +7135,7 @@
         <v>137</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>139</v>
@@ -7185,7 +7188,7 @@
         <v>19</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -7209,7 +7212,7 @@
         <v>19</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>19</v>
@@ -7220,14 +7223,14 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7249,10 +7252,10 @@
         <v>136</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>139</v>
@@ -7307,7 +7310,7 @@
         <v>19</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
@@ -7342,10 +7345,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7368,19 +7371,19 @@
         <v>91</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="O47" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>19</v>
@@ -7405,13 +7408,13 @@
         <v>19</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>19</v>
@@ -7429,7 +7432,7 @@
         <v>19</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>90</v>
@@ -7447,16 +7450,16 @@
         <v>19</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AP47" t="s" s="2">
         <v>19</v>
@@ -7464,10 +7467,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7490,19 +7493,19 @@
         <v>91</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>19</v>
@@ -7551,7 +7554,7 @@
         <v>19</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -7569,27 +7572,27 @@
         <v>19</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP48" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7612,19 +7615,19 @@
         <v>19</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>19</v>
@@ -7649,13 +7652,13 @@
         <v>19</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>19</v>
@@ -7673,7 +7676,7 @@
         <v>19</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7682,7 +7685,7 @@
         <v>90</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>102</v>
@@ -7697,7 +7700,7 @@
         <v>133</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>19</v>
@@ -7708,14 +7711,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7734,19 +7737,19 @@
         <v>19</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>19</v>
@@ -7771,13 +7774,13 @@
         <v>19</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>19</v>
@@ -7795,7 +7798,7 @@
         <v>19</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7813,27 +7816,27 @@
         <v>19</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>19</v>
       </c>
       <c r="AP50" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7859,16 +7862,16 @@
         <v>80</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="O51" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>19</v>
@@ -7917,7 +7920,7 @@
         <v>19</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>78</v>
@@ -7938,10 +7941,10 @@
         <v>19</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>19</v>

</xml_diff>